<commit_message>
Getting Form type improved
</commit_message>
<xml_diff>
--- a/input/Book1.xlsx
+++ b/input/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phdcp\repositories\form-automation\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE748652-972A-43D9-99D4-B4F1E6F1D9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1C5CEF-EEE0-4346-BA58-AC9CC3E7F17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{194A75D5-7A9B-4B69-A8DF-D8D7BE83F330}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{194A75D5-7A9B-4B69-A8DF-D8D7BE83F330}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,10 @@
     <t>Argentina</t>
   </si>
   <si>
-    <t>form_1</t>
-  </si>
-  <si>
     <t>TYPE</t>
+  </si>
+  <si>
+    <t>PERMANENT FOOD FACILITY</t>
   </si>
 </sst>
 </file>
@@ -427,22 +427,23 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>